<commit_message>
Added Multiplicate calculations and evaluation
</commit_message>
<xml_diff>
--- a/Test Case - 1/TC1Results_F.xlsx
+++ b/Test Case - 1/TC1Results_F.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TC1Results_F" sheetId="1" r:id="rId1"/>
+    <sheet name="Reductive" sheetId="1" r:id="rId1"/>
+    <sheet name="Multiplicative" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="82">
   <si>
     <t>d28da70a-3703-47cd-9ee6-75fe92216937</t>
   </si>
@@ -202,6 +203,69 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>XL Multi</t>
+  </si>
+  <si>
+    <t>JSON Multi</t>
+  </si>
+  <si>
+    <t>VSCode Multi</t>
+  </si>
+  <si>
+    <t>Equation 3</t>
+  </si>
+  <si>
+    <t>Equation 4</t>
+  </si>
+  <si>
+    <t>Equation 5</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>a21a66ae-15c0-4ffd-affd-aebcd7411212</t>
+  </si>
+  <si>
+    <t>7e622dce-1a37-4fe7-b293-479091819bf9</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>b07eaf08-c35e-4d47-a6f2-198c9dcbd159</t>
+  </si>
+  <si>
+    <t>99663ee1-da48-46be-95f6-7a7a2c9deea2</t>
+  </si>
+  <si>
+    <t>35c727aa-13d9-486d-ad18-0dcc29b41da4</t>
+  </si>
+  <si>
+    <t>e25facbe-14b6-41c0-a49a-25e11902a0bc</t>
+  </si>
+  <si>
+    <t>2c7f804f-d7ba-42ca-ac41-e253f4abe25f</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>VSCode Match</t>
+  </si>
+  <si>
+    <t>XL Match</t>
   </si>
 </sst>
 </file>
@@ -694,7 +758,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -702,6 +766,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -716,6 +783,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -763,7 +842,58 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1041,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,52 +1181,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
         <v>58</v>
       </c>
@@ -1115,20 +1245,20 @@
       <c r="G2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="5" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2873,6 +3003,3073 @@
       </c>
       <c r="R46" t="s">
         <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="L3:L46">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-2E-3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>10.151999999999999</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>3.6549150560000001</v>
+      </c>
+      <c r="J3">
+        <v>3.6546302110986399</v>
+      </c>
+      <c r="K3">
+        <v>3.68704974301972</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4">
+        <v>3.68704974301972</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" t="b">
+        <f t="shared" ref="R3:R10" si="0">IF(OR(J3*0.95&gt;I3,J3*1.05&gt;I3),TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="S3" t="b">
+        <f>IF(AND(K3&gt;(J3*0.97),K3&lt;(J3*1.03)),TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="T3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
+        <v>20.035</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>10.151999999999999</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2.5475366190000002</v>
+      </c>
+      <c r="J4">
+        <v>2.5473705843182</v>
+      </c>
+      <c r="K4">
+        <v>2.5602306254460698</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="4">
+        <v>2.5602306254460698</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <f t="shared" ref="S4:S50" si="1">IF(AND(K4&gt;(J4*0.97),K4&lt;(J4*1.03)),TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="T4" t="b">
+        <f t="shared" ref="T4:T50" si="2">OR(R4,S4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>20.041</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10.151999999999999</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2.5475366190000002</v>
+      </c>
+      <c r="J5">
+        <v>2.5473705843182</v>
+      </c>
+      <c r="K5">
+        <v>2.5602306254460698</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1</v>
+      </c>
+      <c r="P5" s="4">
+        <v>2.5602306254460698</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S5" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T5" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3">
+        <v>60</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>35.033000000000001</v>
+      </c>
+      <c r="F6" s="3">
+        <v>60.029000000000003</v>
+      </c>
+      <c r="G6" s="3">
+        <v>10.151999999999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>2.5475366190000002</v>
+      </c>
+      <c r="J6">
+        <v>2.5473705843182</v>
+      </c>
+      <c r="K6">
+        <v>2.5602306254460698</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2.5602306254460698</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S6" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T6" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3">
+        <v>60.015999999999998</v>
+      </c>
+      <c r="F7" s="3">
+        <v>35.015000000000001</v>
+      </c>
+      <c r="G7" s="3">
+        <v>10.151999999999999</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>2.5475366190000002</v>
+      </c>
+      <c r="J7">
+        <v>2.5473705843182</v>
+      </c>
+      <c r="K7">
+        <v>2.5602306254460698</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4">
+        <v>1</v>
+      </c>
+      <c r="P7" s="4">
+        <v>2.5602306254460698</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S7" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T7" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>46.3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8">
+        <v>3.2563229050000002</v>
+      </c>
+      <c r="J8">
+        <v>3.2560808244408301</v>
+      </c>
+      <c r="K8">
+        <v>3.2562386816161601</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1</v>
+      </c>
+      <c r="P8" s="4">
+        <v>3.2562386816161601</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>40.015000000000001</v>
+      </c>
+      <c r="G9" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>5.6224755960000001</v>
+      </c>
+      <c r="J9">
+        <v>5.6219796512296698</v>
+      </c>
+      <c r="K9">
+        <v>5.6503853579705599</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="P9" s="4">
+        <v>5.6503853579705599</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S9" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T9" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="F10" s="3">
+        <v>40</v>
+      </c>
+      <c r="G10" s="3">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10">
+        <v>5.203719617</v>
+      </c>
+      <c r="J10">
+        <v>4.7256047977727702</v>
+      </c>
+      <c r="K10">
+        <v>4.7259361688267703</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2.5473922373184399</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N10" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1.32514680800495</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S10" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3">
+        <v>20.024999999999999</v>
+      </c>
+      <c r="F11" s="3">
+        <v>40.021000000000001</v>
+      </c>
+      <c r="G11" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>6.5412467589999999</v>
+      </c>
+      <c r="J11">
+        <v>5.8338908293101799</v>
+      </c>
+      <c r="K11">
+        <v>5.8857634869174698</v>
+      </c>
+      <c r="L11" s="4">
+        <v>3.6868993426302099</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1.2049999999999901</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1.32481268745541</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R11" t="b">
+        <f>IF(OR(J11*0.95&gt;I11,J11*1.05&gt;I11),TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T11" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45</v>
+      </c>
+      <c r="D12" s="3">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3">
+        <v>43.3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12">
+        <v>5.203719617</v>
+      </c>
+      <c r="J12">
+        <v>4.7256047977727702</v>
+      </c>
+      <c r="K12">
+        <v>4.7259361688267703</v>
+      </c>
+      <c r="L12" s="4">
+        <v>2.5473922373184399</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P12" s="4">
+        <v>1.32514680800495</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R12" t="b">
+        <f t="shared" ref="R12:R50" si="3">IF(OR(J12*0.95&gt;I12,J12*1.05&gt;I12),TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T12" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3">
+        <v>55</v>
+      </c>
+      <c r="D13" s="3">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3">
+        <v>19.997</v>
+      </c>
+      <c r="F13" s="3">
+        <v>55.003999999999998</v>
+      </c>
+      <c r="G13" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>5.203719617</v>
+      </c>
+      <c r="J13">
+        <v>4.7244143077676704</v>
+      </c>
+      <c r="K13">
+        <v>4.7483944478399902</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2.560143295729</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P13" s="4">
+        <v>1.32481268745541</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R13" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S13" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T13" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45</v>
+      </c>
+      <c r="C14" s="3">
+        <v>60</v>
+      </c>
+      <c r="D14" s="3">
+        <v>20</v>
+      </c>
+      <c r="E14" s="3">
+        <v>45.015999999999998</v>
+      </c>
+      <c r="F14" s="3">
+        <v>60.015000000000001</v>
+      </c>
+      <c r="G14" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>3.2563229050000002</v>
+      </c>
+      <c r="J14">
+        <v>3.2560808244408301</v>
+      </c>
+      <c r="K14">
+        <v>3.2655507702725499</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
+      <c r="P14" s="4">
+        <v>3.2655507702725499</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R14" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S14" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T14" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3">
+        <v>60</v>
+      </c>
+      <c r="D15" s="3">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3">
+        <v>40.014000000000003</v>
+      </c>
+      <c r="F15" s="3">
+        <v>60.04</v>
+      </c>
+      <c r="G15" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <v>5.6224755960000001</v>
+      </c>
+      <c r="J15">
+        <v>5.6219796512296698</v>
+      </c>
+      <c r="K15">
+        <v>5.6503853579705599</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="4">
+        <v>1</v>
+      </c>
+      <c r="P15" s="4">
+        <v>5.6503853579705599</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T15" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3">
+        <v>50</v>
+      </c>
+      <c r="D16" s="3">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3">
+        <v>40.020000000000003</v>
+      </c>
+      <c r="F16" s="3">
+        <v>50.029000000000003</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>5.203719617</v>
+      </c>
+      <c r="J16">
+        <v>4.7244143077676704</v>
+      </c>
+      <c r="K16">
+        <v>4.7483944478399902</v>
+      </c>
+      <c r="L16" s="4">
+        <v>2.560143295729</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N16" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P16" s="4">
+        <v>1.32481268745541</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R16" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S16" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T16" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>40</v>
+      </c>
+      <c r="C17" s="3">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3">
+        <v>40.002000000000002</v>
+      </c>
+      <c r="F17" s="3">
+        <v>39.994999999999997</v>
+      </c>
+      <c r="G17" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17">
+        <v>6.5412467589999999</v>
+      </c>
+      <c r="J17">
+        <v>5.8338908293101799</v>
+      </c>
+      <c r="K17">
+        <v>5.8857634869174698</v>
+      </c>
+      <c r="L17" s="4">
+        <v>3.6868993426302099</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1.2049999999999901</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1.32481268745541</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R17" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S17" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T17" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3">
+        <v>40</v>
+      </c>
+      <c r="D18" s="3">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3">
+        <v>50.027000000000001</v>
+      </c>
+      <c r="F18" s="3">
+        <v>40.018000000000001</v>
+      </c>
+      <c r="G18" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18">
+        <v>5.203719617</v>
+      </c>
+      <c r="J18">
+        <v>4.7244143077676704</v>
+      </c>
+      <c r="K18">
+        <v>4.7483944478399902</v>
+      </c>
+      <c r="L18" s="4">
+        <v>2.560143295729</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P18" s="4">
+        <v>1.32481268745541</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R18" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S18" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T18" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>60</v>
+      </c>
+      <c r="C19" s="3">
+        <v>40</v>
+      </c>
+      <c r="D19" s="3">
+        <v>20</v>
+      </c>
+      <c r="E19" s="3">
+        <v>60.024000000000001</v>
+      </c>
+      <c r="F19" s="3">
+        <v>40.000999999999998</v>
+      </c>
+      <c r="G19" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <v>5.6224755960000001</v>
+      </c>
+      <c r="J19">
+        <v>5.6219796512296698</v>
+      </c>
+      <c r="K19">
+        <v>5.6503853579705599</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4">
+        <v>5.6503853579705599</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R19" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S19" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T19" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>60</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45</v>
+      </c>
+      <c r="D20" s="3">
+        <v>20</v>
+      </c>
+      <c r="E20" s="3">
+        <v>60.058</v>
+      </c>
+      <c r="F20" s="3">
+        <v>45.052</v>
+      </c>
+      <c r="G20" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20">
+        <v>3.2563229050000002</v>
+      </c>
+      <c r="J20">
+        <v>3.2560808244408301</v>
+      </c>
+      <c r="K20">
+        <v>3.2655507702725499</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1</v>
+      </c>
+      <c r="P20" s="4">
+        <v>3.2655507702725499</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R20" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S20" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T20" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3">
+        <v>50</v>
+      </c>
+      <c r="C21" s="3">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3">
+        <v>20</v>
+      </c>
+      <c r="E21" s="3">
+        <v>49.997</v>
+      </c>
+      <c r="F21" s="3">
+        <v>20.004000000000001</v>
+      </c>
+      <c r="G21" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21">
+        <v>5.203719617</v>
+      </c>
+      <c r="J21">
+        <v>4.7244143077676704</v>
+      </c>
+      <c r="K21">
+        <v>4.7483944478399902</v>
+      </c>
+      <c r="L21" s="4">
+        <v>2.560143295729</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N21" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P21" s="4">
+        <v>1.32481268745541</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R21" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S21" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T21" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3">
+        <v>40</v>
+      </c>
+      <c r="C22" s="3">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3">
+        <v>20</v>
+      </c>
+      <c r="E22" s="3">
+        <v>40.002000000000002</v>
+      </c>
+      <c r="F22" s="3">
+        <v>19.997</v>
+      </c>
+      <c r="G22" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22">
+        <v>6.5412467589999999</v>
+      </c>
+      <c r="J22">
+        <v>5.8338908293101799</v>
+      </c>
+      <c r="K22">
+        <v>5.8857634869174698</v>
+      </c>
+      <c r="L22" s="4">
+        <v>3.6868993426302099</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" s="4">
+        <v>1.2049999999999901</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P22" s="4">
+        <v>1.32481268745541</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R22" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S22" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T22" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3">
+        <v>40</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3">
+        <v>20</v>
+      </c>
+      <c r="E23" s="3">
+        <v>40.003</v>
+      </c>
+      <c r="F23" s="3">
+        <v>9.9990000000000006</v>
+      </c>
+      <c r="G23" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23">
+        <v>5.203719617</v>
+      </c>
+      <c r="J23">
+        <v>4.7244143077676704</v>
+      </c>
+      <c r="K23">
+        <v>4.7483944478399902</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2.560143295729</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N23" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P23" s="4">
+        <v>1.32481268745541</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R23" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S23" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T23" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>20</v>
+      </c>
+      <c r="E24" s="3">
+        <v>40.000999999999998</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="G24" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24">
+        <v>5.6224755960000001</v>
+      </c>
+      <c r="J24">
+        <v>5.6219796512296698</v>
+      </c>
+      <c r="K24">
+        <v>5.6503853579705599</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
+      <c r="N24" s="4">
+        <v>1</v>
+      </c>
+      <c r="P24" s="4">
+        <v>5.6503853579705599</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R24" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S24" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T24" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>20</v>
+      </c>
+      <c r="E25" s="3">
+        <v>45.009</v>
+      </c>
+      <c r="F25" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G25" s="3">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25">
+        <v>3.2563229050000002</v>
+      </c>
+      <c r="J25">
+        <v>3.2560808244408301</v>
+      </c>
+      <c r="K25">
+        <v>3.2655507702725499</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1</v>
+      </c>
+      <c r="P25" s="4">
+        <v>3.2655507702725499</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R25" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S25" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T25" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3">
+        <v>60</v>
+      </c>
+      <c r="D26" s="3">
+        <v>30</v>
+      </c>
+      <c r="E26" s="3">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F26" s="3">
+        <v>59.994999999999997</v>
+      </c>
+      <c r="G26" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26">
+        <v>7.393631976</v>
+      </c>
+      <c r="J26">
+        <v>7.3929459086684801</v>
+      </c>
+      <c r="K26">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="L26" s="4">
+        <v>1</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1</v>
+      </c>
+      <c r="P26" s="4">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R26" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S26" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T26" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>55</v>
+      </c>
+      <c r="D27" s="3">
+        <v>30</v>
+      </c>
+      <c r="E27" s="3">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="F27" s="3">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="G27" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27">
+        <v>3.813163002</v>
+      </c>
+      <c r="J27">
+        <v>3.81286114959329</v>
+      </c>
+      <c r="K27">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="L27" s="4">
+        <v>1</v>
+      </c>
+      <c r="N27" s="4">
+        <v>1</v>
+      </c>
+      <c r="P27" s="4">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R27" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S27" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T27" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>50</v>
+      </c>
+      <c r="D28" s="3">
+        <v>30</v>
+      </c>
+      <c r="E28" s="3">
+        <v>-2E-3</v>
+      </c>
+      <c r="F28" s="3">
+        <v>49.996000000000002</v>
+      </c>
+      <c r="G28" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28">
+        <v>7.393631976</v>
+      </c>
+      <c r="J28">
+        <v>7.3929459086684801</v>
+      </c>
+      <c r="K28">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1</v>
+      </c>
+      <c r="P28" s="4">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R28" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S28" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T28" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>50</v>
+      </c>
+      <c r="D29" s="3">
+        <v>30</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="F29" s="3">
+        <v>49.994</v>
+      </c>
+      <c r="G29" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29">
+        <v>7.1035505069999996</v>
+      </c>
+      <c r="J29">
+        <v>7.1005578156573002</v>
+      </c>
+      <c r="K29">
+        <v>7.1226764402861402</v>
+      </c>
+      <c r="L29" s="4">
+        <v>3.9113927257375201</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N29" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P29" s="4">
+        <v>1.3007198165754299</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R29" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S29" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T29" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3">
+        <v>50</v>
+      </c>
+      <c r="D30" s="3">
+        <v>30</v>
+      </c>
+      <c r="E30" s="3">
+        <v>9.9960000000000004</v>
+      </c>
+      <c r="F30" s="3">
+        <v>49.994999999999997</v>
+      </c>
+      <c r="G30" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H30" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30">
+        <v>10.88167612</v>
+      </c>
+      <c r="J30">
+        <v>10.877006112288599</v>
+      </c>
+      <c r="K30">
+        <v>10.934070163092599</v>
+      </c>
+      <c r="L30" s="4">
+        <v>6.9760735803078102</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N30" s="4">
+        <v>1.2049999999999901</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P30" s="4">
+        <v>1.3007198165754299</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R30" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S30" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T30" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3">
+        <v>10</v>
+      </c>
+      <c r="C31" s="3">
+        <v>55</v>
+      </c>
+      <c r="D31" s="3">
+        <v>30</v>
+      </c>
+      <c r="E31" s="3">
+        <v>9.9969999999999999</v>
+      </c>
+      <c r="F31" s="3">
+        <v>54.994999999999997</v>
+      </c>
+      <c r="G31" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31">
+        <v>7.1035505069999996</v>
+      </c>
+      <c r="J31">
+        <v>7.1005578156573002</v>
+      </c>
+      <c r="K31">
+        <v>7.1226764402861402</v>
+      </c>
+      <c r="L31" s="4">
+        <v>3.9113927257375201</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N31" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P31" s="4">
+        <v>1.3007198165754299</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R31" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S31" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T31" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3">
+        <v>60</v>
+      </c>
+      <c r="D32" s="3">
+        <v>30</v>
+      </c>
+      <c r="E32" s="3">
+        <v>9.9949999999999992</v>
+      </c>
+      <c r="F32" s="3">
+        <v>59.997</v>
+      </c>
+      <c r="G32" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H32" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32">
+        <v>7.393631976</v>
+      </c>
+      <c r="J32">
+        <v>7.3929459086684801</v>
+      </c>
+      <c r="K32">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1</v>
+      </c>
+      <c r="N32" s="4">
+        <v>1</v>
+      </c>
+      <c r="P32" s="4">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R32" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S32" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T32" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3">
+        <v>5</v>
+      </c>
+      <c r="C33" s="3">
+        <v>60</v>
+      </c>
+      <c r="D33" s="3">
+        <v>30</v>
+      </c>
+      <c r="E33" s="3">
+        <v>4.9980000000000002</v>
+      </c>
+      <c r="F33" s="3">
+        <v>59.997</v>
+      </c>
+      <c r="G33" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33">
+        <v>3.813163002</v>
+      </c>
+      <c r="J33">
+        <v>3.81286114959329</v>
+      </c>
+      <c r="K33">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="L33" s="4">
+        <v>1</v>
+      </c>
+      <c r="N33" s="4">
+        <v>1</v>
+      </c>
+      <c r="P33" s="4">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R33" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S33" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T33" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3">
+        <v>50</v>
+      </c>
+      <c r="C34" s="3">
+        <v>60</v>
+      </c>
+      <c r="D34" s="3">
+        <v>30</v>
+      </c>
+      <c r="E34" s="3">
+        <v>49.997</v>
+      </c>
+      <c r="F34" s="3">
+        <v>59.996000000000002</v>
+      </c>
+      <c r="G34" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34">
+        <v>7.393631976</v>
+      </c>
+      <c r="J34">
+        <v>7.3929459086684801</v>
+      </c>
+      <c r="K34">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1</v>
+      </c>
+      <c r="N34" s="4">
+        <v>1</v>
+      </c>
+      <c r="P34" s="4">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R34" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S34" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T34" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3">
+        <v>50</v>
+      </c>
+      <c r="C35" s="3">
+        <v>55</v>
+      </c>
+      <c r="D35" s="3">
+        <v>30</v>
+      </c>
+      <c r="E35" s="3">
+        <v>49.994999999999997</v>
+      </c>
+      <c r="F35" s="3">
+        <v>54.994999999999997</v>
+      </c>
+      <c r="G35" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H35" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35">
+        <v>7.1035505069999996</v>
+      </c>
+      <c r="J35">
+        <v>7.10055785088504</v>
+      </c>
+      <c r="K35">
+        <v>7.1226764402861402</v>
+      </c>
+      <c r="L35" s="4">
+        <v>3.9113927257375201</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N35" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P35" s="4">
+        <v>1.3007198165754299</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R35" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S35" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T35" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3">
+        <v>50</v>
+      </c>
+      <c r="C36" s="3">
+        <v>50</v>
+      </c>
+      <c r="D36" s="3">
+        <v>30</v>
+      </c>
+      <c r="E36" s="3">
+        <v>49.994999999999997</v>
+      </c>
+      <c r="F36" s="3">
+        <v>49.994999999999997</v>
+      </c>
+      <c r="G36" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H36" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36">
+        <v>10.88167612</v>
+      </c>
+      <c r="J36">
+        <v>10.8770061744065</v>
+      </c>
+      <c r="K36">
+        <v>10.934070163092599</v>
+      </c>
+      <c r="L36" s="4">
+        <v>6.9760735803078102</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N36" s="4">
+        <v>1.2049999999999901</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P36" s="4">
+        <v>1.3007198165754299</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R36" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S36" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T36" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3">
+        <v>55</v>
+      </c>
+      <c r="C37" s="3">
+        <v>50</v>
+      </c>
+      <c r="D37" s="3">
+        <v>30</v>
+      </c>
+      <c r="E37" s="3">
+        <v>54.994999999999997</v>
+      </c>
+      <c r="F37" s="3">
+        <v>49.994</v>
+      </c>
+      <c r="G37" s="3">
+        <v>30.151</v>
+      </c>
+      <c r="H37" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37">
+        <v>7.1035505069999996</v>
+      </c>
+      <c r="J37">
+        <v>7.1005717971526803</v>
+      </c>
+      <c r="K37">
+        <v>7.1225473218491304</v>
+      </c>
+      <c r="L37" s="4">
+        <v>3.91131413226976</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N37" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P37" s="4">
+        <v>1.3007223734209401</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R37" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S37" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T37" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3">
+        <v>60</v>
+      </c>
+      <c r="C38" s="3">
+        <v>50</v>
+      </c>
+      <c r="D38" s="3">
+        <v>30</v>
+      </c>
+      <c r="E38" s="3">
+        <v>59.997</v>
+      </c>
+      <c r="F38" s="3">
+        <v>49.994999999999997</v>
+      </c>
+      <c r="G38" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H38" t="s">
+        <v>36</v>
+      </c>
+      <c r="I38">
+        <v>7.393631976</v>
+      </c>
+      <c r="J38">
+        <v>7.3929459086684801</v>
+      </c>
+      <c r="K38">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="L38" s="4">
+        <v>1</v>
+      </c>
+      <c r="N38" s="4">
+        <v>1</v>
+      </c>
+      <c r="P38" s="4">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="Q38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R38" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S38" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T38" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3">
+        <v>60</v>
+      </c>
+      <c r="C39" s="3">
+        <v>55</v>
+      </c>
+      <c r="D39" s="3">
+        <v>30</v>
+      </c>
+      <c r="E39" s="3">
+        <v>59.996000000000002</v>
+      </c>
+      <c r="F39" s="3">
+        <v>54.994999999999997</v>
+      </c>
+      <c r="G39" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H39" t="s">
+        <v>37</v>
+      </c>
+      <c r="I39">
+        <v>3.813163002</v>
+      </c>
+      <c r="J39">
+        <v>3.81286114959329</v>
+      </c>
+      <c r="K39">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="L39" s="4">
+        <v>1</v>
+      </c>
+      <c r="N39" s="4">
+        <v>1</v>
+      </c>
+      <c r="P39" s="4">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="Q39" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R39" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S39" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T39" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3">
+        <v>60</v>
+      </c>
+      <c r="C40" s="3">
+        <v>60</v>
+      </c>
+      <c r="D40" s="3">
+        <v>30</v>
+      </c>
+      <c r="E40" s="3">
+        <v>59.999000000000002</v>
+      </c>
+      <c r="F40" s="3">
+        <v>59.994</v>
+      </c>
+      <c r="G40" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40">
+        <v>7.393631976</v>
+      </c>
+      <c r="J40">
+        <v>7.3929459086684801</v>
+      </c>
+      <c r="K40">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="L40" s="4">
+        <v>1</v>
+      </c>
+      <c r="N40" s="4">
+        <v>1</v>
+      </c>
+      <c r="P40" s="4">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R40" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S40" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T40" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="3">
+        <v>55</v>
+      </c>
+      <c r="C41" s="3">
+        <v>60</v>
+      </c>
+      <c r="D41" s="3">
+        <v>30</v>
+      </c>
+      <c r="E41" s="3">
+        <v>54.994999999999997</v>
+      </c>
+      <c r="F41" s="3">
+        <v>59.994</v>
+      </c>
+      <c r="G41" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41">
+        <v>3.813163002</v>
+      </c>
+      <c r="J41">
+        <v>3.81286114959329</v>
+      </c>
+      <c r="K41">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="N41" s="4">
+        <v>1</v>
+      </c>
+      <c r="P41" s="4">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R41" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S41" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T41" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3">
+        <v>50</v>
+      </c>
+      <c r="C42" s="3">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3">
+        <v>30</v>
+      </c>
+      <c r="E42" s="3">
+        <v>49.994999999999997</v>
+      </c>
+      <c r="F42" s="3">
+        <v>9.9939999999999998</v>
+      </c>
+      <c r="G42" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H42" t="s">
+        <v>40</v>
+      </c>
+      <c r="I42">
+        <v>10.88167612</v>
+      </c>
+      <c r="J42">
+        <v>10.8770061433476</v>
+      </c>
+      <c r="K42">
+        <v>10.934070163092599</v>
+      </c>
+      <c r="L42" s="4">
+        <v>6.9760735803078102</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N42" s="4">
+        <v>1.2049999999999901</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P42" s="4">
+        <v>1.3007198165754299</v>
+      </c>
+      <c r="Q42" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R42" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S42" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T42" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>41</v>
+      </c>
+      <c r="B43" s="3">
+        <v>50</v>
+      </c>
+      <c r="C43" s="3">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3">
+        <v>30</v>
+      </c>
+      <c r="E43" s="3">
+        <v>49.997999999999998</v>
+      </c>
+      <c r="F43" s="3">
+        <v>4.9960000000000004</v>
+      </c>
+      <c r="G43" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H43" t="s">
+        <v>42</v>
+      </c>
+      <c r="I43">
+        <v>7.1035505069999996</v>
+      </c>
+      <c r="J43">
+        <v>7.1005578332711696</v>
+      </c>
+      <c r="K43">
+        <v>7.1226764402861402</v>
+      </c>
+      <c r="L43" s="4">
+        <v>3.9113927257375201</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N43" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P43" s="4">
+        <v>1.3007198165754299</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R43" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S43" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T43" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3">
+        <v>50</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>30</v>
+      </c>
+      <c r="E44" s="3">
+        <v>49.996000000000002</v>
+      </c>
+      <c r="F44" s="3">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="G44" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H44" t="s">
+        <v>43</v>
+      </c>
+      <c r="I44">
+        <v>7.393631976</v>
+      </c>
+      <c r="J44">
+        <v>7.3929459086684801</v>
+      </c>
+      <c r="K44">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="L44" s="4">
+        <v>1</v>
+      </c>
+      <c r="N44" s="4">
+        <v>1</v>
+      </c>
+      <c r="P44" s="4">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R44" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S44" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T44" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3">
+        <v>55</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
+        <v>30</v>
+      </c>
+      <c r="E45" s="3">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="F45" s="3">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="G45" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H45" t="s">
+        <v>44</v>
+      </c>
+      <c r="I45">
+        <v>3.813163002</v>
+      </c>
+      <c r="J45">
+        <v>3.81286114959329</v>
+      </c>
+      <c r="K45">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1</v>
+      </c>
+      <c r="N45" s="4">
+        <v>1</v>
+      </c>
+      <c r="P45" s="4">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R45" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S45" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T45" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3">
+        <v>60</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>30</v>
+      </c>
+      <c r="E46" s="3">
+        <v>59.996000000000002</v>
+      </c>
+      <c r="F46" s="3">
+        <v>4.9950000000000001</v>
+      </c>
+      <c r="G46" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H46" t="s">
+        <v>45</v>
+      </c>
+      <c r="I46">
+        <v>7.393631976</v>
+      </c>
+      <c r="J46">
+        <v>3.81286114959329</v>
+      </c>
+      <c r="K46">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="L46" s="4">
+        <v>1</v>
+      </c>
+      <c r="N46" s="4">
+        <v>1</v>
+      </c>
+      <c r="P46" s="4">
+        <v>3.8208025962606902</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R46" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S46" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T46" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>45</v>
+      </c>
+      <c r="B47" s="3">
+        <v>60</v>
+      </c>
+      <c r="C47" s="3">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3">
+        <v>30</v>
+      </c>
+      <c r="E47" s="3">
+        <v>60</v>
+      </c>
+      <c r="F47" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="G47" s="3">
+        <v>30</v>
+      </c>
+      <c r="H47" t="s">
+        <v>75</v>
+      </c>
+      <c r="I47">
+        <v>3.813163002</v>
+      </c>
+      <c r="J47">
+        <v>3.81286114959329</v>
+      </c>
+      <c r="K47">
+        <v>3.8130579932127699</v>
+      </c>
+      <c r="L47" s="4">
+        <v>1</v>
+      </c>
+      <c r="N47" s="4">
+        <v>1</v>
+      </c>
+      <c r="P47" s="4">
+        <v>3.8130579932127699</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R47" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S47" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T47" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3">
+        <v>60</v>
+      </c>
+      <c r="C48" s="3">
+        <v>10</v>
+      </c>
+      <c r="D48" s="3">
+        <v>30</v>
+      </c>
+      <c r="E48" s="3">
+        <v>59.996000000000002</v>
+      </c>
+      <c r="F48" s="3">
+        <v>9.9939999999999998</v>
+      </c>
+      <c r="G48" s="3">
+        <v>30.152000000000001</v>
+      </c>
+      <c r="H48" t="s">
+        <v>76</v>
+      </c>
+      <c r="I48">
+        <v>7.393631976</v>
+      </c>
+      <c r="J48">
+        <v>7.3929459086684801</v>
+      </c>
+      <c r="K48">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="L48" s="4">
+        <v>1</v>
+      </c>
+      <c r="N48" s="4">
+        <v>1</v>
+      </c>
+      <c r="P48" s="4">
+        <v>7.4192947675644998</v>
+      </c>
+      <c r="Q48" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R48" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S48" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T48" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>47</v>
+      </c>
+      <c r="B49" s="3">
+        <v>55</v>
+      </c>
+      <c r="C49" s="3">
+        <v>10</v>
+      </c>
+      <c r="D49" s="3">
+        <v>30</v>
+      </c>
+      <c r="E49" s="3">
+        <v>55.2</v>
+      </c>
+      <c r="F49" s="3">
+        <v>10</v>
+      </c>
+      <c r="G49" s="3">
+        <v>30</v>
+      </c>
+      <c r="H49" t="s">
+        <v>77</v>
+      </c>
+      <c r="I49">
+        <v>7.1035505069999996</v>
+      </c>
+      <c r="J49">
+        <v>7.1026763976886</v>
+      </c>
+      <c r="K49">
+        <v>7.10300539885856</v>
+      </c>
+      <c r="L49" s="4">
+        <v>3.8994260342242</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N49" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O49" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P49" s="4">
+        <v>1.30110822474117</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R49" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S49" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T49" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>52</v>
+      </c>
+      <c r="B50" s="3">
+        <v>13.7</v>
+      </c>
+      <c r="C50" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="D50" s="3">
+        <v>10</v>
+      </c>
+      <c r="E50" s="3">
+        <v>13.7</v>
+      </c>
+      <c r="F50" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="G50" s="3">
+        <v>10</v>
+      </c>
+      <c r="H50" t="s">
+        <v>78</v>
+      </c>
+      <c r="I50">
+        <v>1.341894991</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>1.3418431132513999</v>
+      </c>
+      <c r="L50" s="4">
+        <v>1</v>
+      </c>
+      <c r="N50" s="4">
+        <v>1</v>
+      </c>
+      <c r="P50" s="4">
+        <v>1.3418431132513999</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="R50" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S50" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T50" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2883,14 +6080,30 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="T1:T2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
+  <conditionalFormatting sqref="T3:T50">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3:S50">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor update to proper pulled points
</commit_message>
<xml_diff>
--- a/Test Case - 1/TC1Results_F.xlsx
+++ b/Test Case - 1/TC1Results_F.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="80">
   <si>
     <t>d28da70a-3703-47cd-9ee6-75fe92216937</t>
   </si>
@@ -254,12 +254,6 @@
   </si>
   <si>
     <t>e25facbe-14b6-41c0-a49a-25e11902a0bc</t>
-  </si>
-  <si>
-    <t>2c7f804f-d7ba-42ca-ac41-e253f4abe25f</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t>VSCode Match</t>
@@ -786,9 +780,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -796,6 +787,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3007,6 +3001,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
@@ -3014,12 +3014,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L46">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
@@ -3032,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3046,55 +3040,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="12" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="11" t="s">
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="T1" s="10" t="s">
-        <v>80</v>
+      <c r="T1" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="3" t="s">
         <v>58</v>
       </c>
@@ -3113,19 +3107,19 @@
       <c r="G2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="13"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -3236,11 +3230,11 @@
         <v>1</v>
       </c>
       <c r="S4" t="b">
-        <f t="shared" ref="S4:S50" si="1">IF(AND(K4&gt;(J4*0.97),K4&lt;(J4*1.03)),TRUE,FALSE)</f>
+        <f t="shared" ref="S4:S49" si="1">IF(AND(K4&gt;(J4*0.97),K4&lt;(J4*1.03)),TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="T4" t="b">
-        <f t="shared" ref="T4:T50" si="2">OR(R4,S4)</f>
+        <f t="shared" ref="T4:T49" si="2">OR(R4,S4)</f>
         <v>1</v>
       </c>
     </row>
@@ -3722,7 +3716,7 @@
         <v>72</v>
       </c>
       <c r="R12" t="b">
-        <f t="shared" ref="R12:R50" si="3">IF(OR(J12*0.95&gt;I12,J12*1.05&gt;I12),TRUE,FALSE)</f>
+        <f t="shared" ref="R12:R49" si="3">IF(OR(J12*0.95&gt;I12,J12*1.05&gt;I12),TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="S12" t="b">
@@ -6013,73 +6007,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>52</v>
-      </c>
-      <c r="B50" s="3">
-        <v>13.7</v>
-      </c>
-      <c r="C50" s="3">
-        <v>10.7</v>
-      </c>
-      <c r="D50" s="3">
-        <v>10</v>
-      </c>
-      <c r="E50" s="3">
-        <v>13.7</v>
-      </c>
-      <c r="F50" s="3">
-        <v>10.7</v>
-      </c>
-      <c r="G50" s="3">
-        <v>10</v>
-      </c>
-      <c r="H50" t="s">
-        <v>78</v>
-      </c>
-      <c r="I50">
-        <v>1.341894991</v>
-      </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>1.3418431132513999</v>
-      </c>
-      <c r="L50" s="4">
-        <v>1</v>
-      </c>
-      <c r="N50" s="4">
-        <v>1</v>
-      </c>
-      <c r="P50" s="4">
-        <v>1.3418431132513999</v>
-      </c>
-      <c r="Q50" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="R50" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S50" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T50" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:M2"/>
@@ -6087,8 +6016,14 @@
     <mergeCell ref="P1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
-  <conditionalFormatting sqref="T3:T50">
+  <conditionalFormatting sqref="T3:T49">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -6096,7 +6031,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:S50">
+  <conditionalFormatting sqref="R3:S49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>